<commit_message>
Adding User in Herokuapp TC to add the users given in excel file.
</commit_message>
<xml_diff>
--- a/SeleniumExamples/src/main/config/excelDataFiles/HerokuappData.xlsx
+++ b/SeleniumExamples/src/main/config/excelDataFiles/HerokuappData.xlsx
@@ -1971,7 +1971,7 @@
         <v>45</v>
       </c>
       <c r="E6" s="1">
-        <v>4.47529887644E11</v>
+        <v>7.529887644E9</v>
       </c>
       <c r="F6" s="1" t="s">
         <v>46</v>
@@ -2146,7 +2146,7 @@
         <v>80</v>
       </c>
       <c r="E11" s="1">
-        <v>4.42071838299E11</v>
+        <v>2.071838299E9</v>
       </c>
       <c r="F11" s="1" t="s">
         <v>81</v>
@@ -2706,7 +2706,7 @@
         <v>179</v>
       </c>
       <c r="E27" s="1">
-        <v>4.4756388321E11</v>
+        <v>7.56388321E9</v>
       </c>
       <c r="F27" s="1" t="s">
         <v>180</v>
@@ -2986,7 +2986,7 @@
         <v>225</v>
       </c>
       <c r="E35" s="1">
-        <v>4.41632960123E11</v>
+        <v>1.632960123E9</v>
       </c>
       <c r="F35" s="1" t="s">
         <v>226</v>
@@ -3476,7 +3476,7 @@
         <v>301</v>
       </c>
       <c r="E49" s="1">
-        <v>4.47592881234E11</v>
+        <v>7.592881234E9</v>
       </c>
       <c r="F49" s="1" t="s">
         <v>302</v>
@@ -3826,7 +3826,7 @@
         <v>353</v>
       </c>
       <c r="E59" s="1">
-        <v>4.47523990099E11</v>
+        <v>7.523990099E9</v>
       </c>
       <c r="F59" s="1" t="s">
         <v>354</v>
@@ -4806,7 +4806,7 @@
         <v>479</v>
       </c>
       <c r="E87" s="1">
-        <v>4.47563882199E11</v>
+        <v>7.563882199E9</v>
       </c>
       <c r="F87" s="1" t="s">
         <v>480</v>

</xml_diff>